<commit_message>
Sorted valid min and max for lux qc processing
</commit_message>
<xml_diff>
--- a/specific_variables/flux-components-level1.xlsx
+++ b/specific_variables/flux-components-level1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310932DC-C5A2-0445-A145-4A7F900018A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69247401-756D-194A-B4BC-C42E5B95B7E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29200" yWindow="-2460" windowWidth="17100" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7180" yWindow="460" windowWidth="21480" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="179">
   <si>
     <t>Variable</t>
   </si>
@@ -973,8 +973,8 @@
   </sheetPr>
   <dimension ref="A1:C961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A678" workbookViewId="0">
-      <selection activeCell="C711" sqref="A1:C711"/>
+    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
+      <selection activeCell="A560" sqref="A560:C561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4344,1786 +4344,1834 @@
       </c>
     </row>
     <row r="461" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B461" t="s">
+      <c r="A461" s="8"/>
+      <c r="B461" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C461" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A462" s="8"/>
+      <c r="B462" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C462" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B463" t="s">
         <v>26</v>
       </c>
-      <c r="C461" t="s">
+      <c r="C463" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="462" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B462" t="s">
+    <row r="464" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B464" t="s">
         <v>16</v>
       </c>
-      <c r="C462" t="s">
+      <c r="C464" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="463" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A464" t="s">
+    <row r="465" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A466" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="465" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B465" t="s">
-        <v>5</v>
-      </c>
-      <c r="C465" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="466" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B466" t="s">
-        <v>7</v>
-      </c>
-      <c r="C466" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="467" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B467" t="s">
-        <v>3</v>
-      </c>
-      <c r="C467" s="4" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="C467" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="468" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B468" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C468" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="469" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B469" t="s">
+        <v>3</v>
+      </c>
+      <c r="C469" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B470" t="s">
+        <v>11</v>
+      </c>
+      <c r="C470" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B471" t="s">
         <v>13</v>
       </c>
-      <c r="C469" s="3">
+      <c r="C471" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A470" s="8"/>
-      <c r="B470" s="8" t="s">
+    <row r="472" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A472" s="8"/>
+      <c r="B472" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C470" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="471" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A471" s="8"/>
-      <c r="B471" s="8" t="s">
+      <c r="C472" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A473" s="8"/>
+      <c r="B473" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C471" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="472" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B472" t="s">
+      <c r="C473" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B474" t="s">
         <v>26</v>
       </c>
-      <c r="C472" t="s">
+      <c r="C474" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B473" t="s">
+    <row r="475" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B475" t="s">
         <v>16</v>
       </c>
-      <c r="C473" t="s">
+      <c r="C475" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="474" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A475" t="s">
+    <row r="476" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A477" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="476" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B476" t="s">
-        <v>5</v>
-      </c>
-      <c r="C476" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B477" t="s">
-        <v>7</v>
-      </c>
-      <c r="C477" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="478" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B478" t="s">
-        <v>3</v>
-      </c>
-      <c r="C478" s="4" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="C478" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="479" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B479" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C479" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
     </row>
     <row r="480" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B480" t="s">
+        <v>3</v>
+      </c>
+      <c r="C480" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B481" t="s">
+        <v>11</v>
+      </c>
+      <c r="C481" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B482" t="s">
         <v>13</v>
       </c>
-      <c r="C480" s="3">
+      <c r="C482" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="481" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A481" s="8"/>
-      <c r="B481" s="8" t="s">
+    <row r="483" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A483" s="8"/>
+      <c r="B483" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C481" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="482" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A482" s="8"/>
-      <c r="B482" s="8" t="s">
+      <c r="C483" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A484" s="8"/>
+      <c r="B484" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C482" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="483" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B483" t="s">
+      <c r="C484" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B485" t="s">
         <v>26</v>
       </c>
-      <c r="C483" t="s">
+      <c r="C485" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="484" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B484" t="s">
+    <row r="486" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B486" t="s">
         <v>16</v>
       </c>
-      <c r="C484" t="s">
+      <c r="C486" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="485" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A486" t="s">
+    <row r="487" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A488" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="487" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B487" t="s">
-        <v>5</v>
-      </c>
-      <c r="C487" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="488" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B488" t="s">
-        <v>7</v>
-      </c>
-      <c r="C488" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="489" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B489" t="s">
-        <v>3</v>
-      </c>
-      <c r="C489" s="4" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="C489" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="490" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B490" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C490" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
     </row>
     <row r="491" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B491" t="s">
+        <v>3</v>
+      </c>
+      <c r="C491" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B492" t="s">
+        <v>11</v>
+      </c>
+      <c r="C492" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B493" t="s">
         <v>13</v>
       </c>
-      <c r="C491" s="3">
+      <c r="C493" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="492" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A492" s="8"/>
-      <c r="B492" s="8" t="s">
+    <row r="494" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A494" s="8"/>
+      <c r="B494" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C492" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="493" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A493" s="8"/>
-      <c r="B493" s="8" t="s">
+      <c r="C494" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A495" s="8"/>
+      <c r="B495" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C493" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="494" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B494" t="s">
+      <c r="C495" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B496" t="s">
         <v>26</v>
       </c>
-      <c r="C494" t="s">
+      <c r="C496" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="495" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B495" t="s">
+    <row r="497" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B497" t="s">
         <v>16</v>
       </c>
-      <c r="C495" t="s">
+      <c r="C497" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="496" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A497" t="s">
+    <row r="498" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A499" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="498" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B498" t="s">
-        <v>5</v>
-      </c>
-      <c r="C498" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="499" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B499" t="s">
-        <v>7</v>
-      </c>
-      <c r="C499" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="500" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B500" t="s">
-        <v>3</v>
-      </c>
-      <c r="C500" s="4" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="C500" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="501" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B501" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C501" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
     </row>
     <row r="502" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B502" t="s">
+        <v>3</v>
+      </c>
+      <c r="C502" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B503" t="s">
+        <v>11</v>
+      </c>
+      <c r="C503" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B504" t="s">
         <v>13</v>
       </c>
-      <c r="C502" s="3">
+      <c r="C504" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="503" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A503" s="8"/>
-      <c r="B503" s="8" t="s">
+    <row r="505" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A505" s="8"/>
+      <c r="B505" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C503" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="504" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A504" s="8"/>
-      <c r="B504" s="8" t="s">
+      <c r="C505" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A506" s="8"/>
+      <c r="B506" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C504" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="505" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B505" t="s">
+      <c r="C506" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B507" t="s">
         <v>26</v>
       </c>
-      <c r="C505" t="s">
+      <c r="C507" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="506" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B506" t="s">
+    <row r="508" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B508" t="s">
         <v>16</v>
       </c>
-      <c r="C506" t="s">
+      <c r="C508" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="507" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A508" t="s">
+    <row r="509" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A510" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="509" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B509" t="s">
-        <v>5</v>
-      </c>
-      <c r="C509" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="510" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B510" t="s">
-        <v>7</v>
-      </c>
-      <c r="C510" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="511" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B511" t="s">
-        <v>3</v>
-      </c>
-      <c r="C511" s="4" t="s">
-        <v>123</v>
+        <v>5</v>
+      </c>
+      <c r="C511" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="512" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B512" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C512" t="s">
-        <v>124</v>
+        <v>24</v>
       </c>
     </row>
     <row r="513" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B513" t="s">
+        <v>3</v>
+      </c>
+      <c r="C513" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B514" t="s">
+        <v>11</v>
+      </c>
+      <c r="C514" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B515" t="s">
         <v>13</v>
       </c>
-      <c r="C513" s="3">
+      <c r="C515" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="514" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A514" s="8"/>
-      <c r="B514" s="8" t="s">
+    <row r="516" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A516" s="8"/>
+      <c r="B516" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C514" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="515" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A515" s="8"/>
-      <c r="B515" s="8" t="s">
+      <c r="C516" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A517" s="8"/>
+      <c r="B517" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C515" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="516" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B516" t="s">
+      <c r="C517" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B518" t="s">
         <v>26</v>
       </c>
-      <c r="C516" t="s">
+      <c r="C518" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="517" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B517" t="s">
+    <row r="519" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B519" t="s">
         <v>16</v>
       </c>
-      <c r="C517" t="s">
+      <c r="C519" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="518" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A519" t="s">
+    <row r="520" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A521" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="520" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B520" t="s">
-        <v>5</v>
-      </c>
-      <c r="C520" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="521" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B521" t="s">
-        <v>7</v>
-      </c>
-      <c r="C521" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="522" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B522" t="s">
-        <v>3</v>
-      </c>
-      <c r="C522" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
+      </c>
+      <c r="C522" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="523" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B523" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C523" t="s">
-        <v>127</v>
+        <v>24</v>
       </c>
     </row>
     <row r="524" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B524" t="s">
+        <v>3</v>
+      </c>
+      <c r="C524" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B525" t="s">
+        <v>11</v>
+      </c>
+      <c r="C525" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B526" t="s">
         <v>13</v>
       </c>
-      <c r="C524" s="3">
+      <c r="C526" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="525" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A525" s="8"/>
-      <c r="B525" s="8" t="s">
+    <row r="527" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A527" s="8"/>
+      <c r="B527" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C525" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="526" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A526" s="8"/>
-      <c r="B526" s="8" t="s">
+      <c r="C527" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A528" s="8"/>
+      <c r="B528" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C526" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="527" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B527" t="s">
+      <c r="C528" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B529" t="s">
         <v>26</v>
       </c>
-      <c r="C527" t="s">
+      <c r="C529" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="528" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B528" t="s">
+    <row r="530" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B530" t="s">
         <v>16</v>
       </c>
-      <c r="C528" t="s">
+      <c r="C530" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="529" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A530" s="2" t="s">
+    <row r="531" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A532" s="2" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="531" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B531" t="s">
-        <v>5</v>
-      </c>
-      <c r="C531" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="532" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B532" t="s">
-        <v>7</v>
-      </c>
-      <c r="C532" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="533" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B533" t="s">
-        <v>3</v>
-      </c>
-      <c r="C533" s="4" t="s">
-        <v>129</v>
+        <v>5</v>
+      </c>
+      <c r="C533" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="534" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B534" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C534" t="s">
-        <v>130</v>
+        <v>24</v>
       </c>
     </row>
     <row r="535" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B535" t="s">
+        <v>3</v>
+      </c>
+      <c r="C535" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B536" t="s">
+        <v>11</v>
+      </c>
+      <c r="C536" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B537" t="s">
         <v>13</v>
       </c>
-      <c r="C535" s="3">
+      <c r="C537" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="536" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A536" s="8"/>
-      <c r="B536" s="8" t="s">
+    <row r="538" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A538" s="8"/>
+      <c r="B538" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C536" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="537" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A537" s="8"/>
-      <c r="B537" s="8" t="s">
+      <c r="C538" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A539" s="8"/>
+      <c r="B539" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C537" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="538" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B538" t="s">
+      <c r="C539" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B540" t="s">
         <v>26</v>
       </c>
-      <c r="C538" t="s">
+      <c r="C540" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="539" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B539" t="s">
+    <row r="541" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B541" t="s">
         <v>16</v>
       </c>
-      <c r="C539" t="s">
+      <c r="C541" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="540" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A541" t="s">
+    <row r="542" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A543" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="542" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B542" t="s">
-        <v>5</v>
-      </c>
-      <c r="C542" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="543" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B543" t="s">
-        <v>7</v>
-      </c>
-      <c r="C543" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="544" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B544" t="s">
-        <v>3</v>
-      </c>
-      <c r="C544" s="4" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="C544" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="545" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B545" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C545" t="s">
-        <v>132</v>
+        <v>8</v>
       </c>
     </row>
     <row r="546" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B546" t="s">
+        <v>3</v>
+      </c>
+      <c r="C546" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B547" t="s">
+        <v>11</v>
+      </c>
+      <c r="C547" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B548" t="s">
         <v>13</v>
       </c>
-      <c r="C546" s="3">
+      <c r="C548" s="3">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="547" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A547" s="8"/>
-      <c r="B547" s="8" t="s">
+    <row r="549" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A549" s="8"/>
+      <c r="B549" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C547" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="548" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A548" s="8"/>
-      <c r="B548" s="8" t="s">
+      <c r="C549" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A550" s="8"/>
+      <c r="B550" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C548" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="549" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B549" t="s">
+      <c r="C550" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B551" t="s">
         <v>26</v>
       </c>
-      <c r="C549" t="s">
+      <c r="C551" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="550" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B550" t="s">
+    <row r="552" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B552" t="s">
         <v>16</v>
       </c>
-      <c r="C550" t="s">
+      <c r="C552" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="551" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A552" t="s">
+    <row r="553" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A554" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="553" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B553" t="s">
-        <v>5</v>
-      </c>
-      <c r="C553" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="554" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B554" t="s">
-        <v>7</v>
-      </c>
-      <c r="C554" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="555" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B555" t="s">
-        <v>3</v>
-      </c>
-      <c r="C555" s="4" t="s">
-        <v>112</v>
+        <v>5</v>
+      </c>
+      <c r="C555" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="556" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B556" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C556" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
     </row>
     <row r="557" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B557" t="s">
-        <v>13</v>
-      </c>
-      <c r="C557" s="3">
-        <v>-1E+20</v>
+        <v>3</v>
+      </c>
+      <c r="C557" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="558" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B558" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C558" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
     </row>
     <row r="559" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B559" t="s">
-        <v>16</v>
-      </c>
-      <c r="C559" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="560" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>13</v>
+      </c>
+      <c r="C559" s="3">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A560" s="8"/>
+      <c r="B560" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C560" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="561" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A561" t="s">
-        <v>135</v>
+      <c r="A561" s="8"/>
+      <c r="B561" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C561" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="562" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B562" t="s">
-        <v>5</v>
-      </c>
-      <c r="C562" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="C562" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="563" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B563" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C563" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="564" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B564" t="s">
-        <v>3</v>
-      </c>
-      <c r="C564" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="565" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B565" t="s">
-        <v>11</v>
-      </c>
-      <c r="C565" t="s">
-        <v>136</v>
+      <c r="A565" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="566" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B566" t="s">
-        <v>13</v>
-      </c>
-      <c r="C566" s="3">
-        <v>-1E+20</v>
+        <v>5</v>
+      </c>
+      <c r="C566" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="567" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A567" s="8"/>
-      <c r="B567" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C567" s="11" t="s">
-        <v>174</v>
+      <c r="B567" t="s">
+        <v>7</v>
+      </c>
+      <c r="C567" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="568" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A568" s="8"/>
-      <c r="B568" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C568" s="11" t="s">
-        <v>174</v>
+      <c r="B568" t="s">
+        <v>3</v>
+      </c>
+      <c r="C568" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="569" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B569" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C569" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
     </row>
     <row r="570" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B570" t="s">
-        <v>16</v>
-      </c>
-      <c r="C570" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="571" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>13</v>
+      </c>
+      <c r="C570" s="3">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A571" s="8"/>
+      <c r="B571" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C571" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="572" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A572" t="s">
-        <v>137</v>
+      <c r="A572" s="8"/>
+      <c r="B572" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C572" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="573" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B573" t="s">
-        <v>5</v>
-      </c>
-      <c r="C573" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="C573" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="574" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B574" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C574" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="575" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B575" t="s">
-        <v>3</v>
-      </c>
-      <c r="C575" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="576" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B576" t="s">
-        <v>11</v>
-      </c>
-      <c r="C576" t="s">
-        <v>138</v>
+      <c r="A576" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="577" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B577" t="s">
-        <v>13</v>
-      </c>
-      <c r="C577" s="3">
-        <v>-1E+20</v>
+        <v>5</v>
+      </c>
+      <c r="C577" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="578" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B578" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C578" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
     </row>
     <row r="579" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B579" t="s">
-        <v>16</v>
-      </c>
-      <c r="C579" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="580" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>3</v>
+      </c>
+      <c r="C579" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B580" t="s">
+        <v>11</v>
+      </c>
+      <c r="C580" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="581" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A581" t="s">
-        <v>139</v>
+      <c r="B581" t="s">
+        <v>13</v>
+      </c>
+      <c r="C581" s="3">
+        <v>-1E+20</v>
       </c>
     </row>
     <row r="582" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B582" t="s">
-        <v>5</v>
-      </c>
-      <c r="C582" s="2" t="s">
-        <v>19</v>
+      <c r="A582" s="8"/>
+      <c r="B582" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C582" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="583" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B583" t="s">
-        <v>7</v>
-      </c>
-      <c r="C583" t="s">
-        <v>8</v>
+      <c r="A583" s="8"/>
+      <c r="B583" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C583" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="584" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B584" t="s">
-        <v>3</v>
-      </c>
-      <c r="C584" s="4" t="s">
-        <v>112</v>
+        <v>26</v>
+      </c>
+      <c r="C584" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="585" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B585" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C585" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="586" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B586" t="s">
-        <v>13</v>
-      </c>
-      <c r="C586" s="3">
-        <v>-1E+20</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="587" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A587" s="8"/>
-      <c r="B587" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C587" s="11" t="s">
-        <v>174</v>
+      <c r="A587" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="588" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A588" s="8"/>
-      <c r="B588" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C588" s="11" t="s">
-        <v>174</v>
+      <c r="B588" t="s">
+        <v>5</v>
+      </c>
+      <c r="C588" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="589" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B589" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C589" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
     </row>
     <row r="590" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B590" t="s">
-        <v>16</v>
-      </c>
-      <c r="C590" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="591" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>3</v>
+      </c>
+      <c r="C590" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B591" t="s">
+        <v>11</v>
+      </c>
+      <c r="C591" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="592" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A592" t="s">
-        <v>141</v>
+      <c r="B592" t="s">
+        <v>13</v>
+      </c>
+      <c r="C592" s="3">
+        <v>-1E+20</v>
       </c>
     </row>
     <row r="593" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B593" t="s">
-        <v>5</v>
-      </c>
-      <c r="C593" s="2" t="s">
-        <v>19</v>
+      <c r="A593" s="8"/>
+      <c r="B593" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C593" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="594" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B594" t="s">
-        <v>7</v>
-      </c>
-      <c r="C594" t="s">
-        <v>8</v>
+      <c r="A594" s="8"/>
+      <c r="B594" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C594" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="595" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B595" t="s">
-        <v>3</v>
-      </c>
-      <c r="C595" s="4" t="s">
-        <v>123</v>
+        <v>26</v>
+      </c>
+      <c r="C595" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="596" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B596" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C596" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="597" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B597" t="s">
-        <v>13</v>
-      </c>
-      <c r="C597" s="3">
-        <v>-1E+20</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="598" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A598" s="8"/>
-      <c r="B598" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C598" s="11" t="s">
-        <v>174</v>
+      <c r="A598" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="599" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A599" s="8"/>
-      <c r="B599" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C599" s="11" t="s">
-        <v>174</v>
+      <c r="B599" t="s">
+        <v>5</v>
+      </c>
+      <c r="C599" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="600" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B600" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C600" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
     </row>
     <row r="601" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B601" t="s">
-        <v>16</v>
-      </c>
-      <c r="C601" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="602" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>3</v>
+      </c>
+      <c r="C601" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B602" t="s">
+        <v>11</v>
+      </c>
+      <c r="C602" t="s">
+        <v>142</v>
+      </c>
+    </row>
     <row r="603" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A603" t="s">
-        <v>143</v>
+      <c r="B603" t="s">
+        <v>13</v>
+      </c>
+      <c r="C603" s="3">
+        <v>-1E+20</v>
       </c>
     </row>
     <row r="604" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B604" t="s">
-        <v>5</v>
-      </c>
-      <c r="C604" s="2" t="s">
-        <v>19</v>
+      <c r="A604" s="8"/>
+      <c r="B604" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C604" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="605" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B605" t="s">
-        <v>7</v>
-      </c>
-      <c r="C605" t="s">
-        <v>8</v>
+      <c r="A605" s="8"/>
+      <c r="B605" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C605" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="606" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B606" t="s">
-        <v>3</v>
-      </c>
-      <c r="C606" s="4" t="s">
-        <v>125</v>
+        <v>26</v>
+      </c>
+      <c r="C606" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="607" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B607" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C607" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="608" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B608" t="s">
-        <v>13</v>
-      </c>
-      <c r="C608" s="3">
-        <v>-1E+20</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="609" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A609" s="8"/>
-      <c r="B609" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C609" s="11" t="s">
-        <v>174</v>
+      <c r="A609" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="610" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A610" s="8"/>
-      <c r="B610" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C610" s="11" t="s">
-        <v>174</v>
+      <c r="B610" t="s">
+        <v>5</v>
+      </c>
+      <c r="C610" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="611" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B611" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C611" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
     </row>
     <row r="612" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B612" t="s">
-        <v>16</v>
-      </c>
-      <c r="C612" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="613" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>3</v>
+      </c>
+      <c r="C612" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B613" t="s">
+        <v>11</v>
+      </c>
+      <c r="C613" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="614" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A614" s="2" t="s">
-        <v>145</v>
+      <c r="B614" t="s">
+        <v>13</v>
+      </c>
+      <c r="C614" s="3">
+        <v>-1E+20</v>
       </c>
     </row>
     <row r="615" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B615" t="s">
-        <v>5</v>
-      </c>
-      <c r="C615" s="2" t="s">
-        <v>19</v>
+      <c r="A615" s="8"/>
+      <c r="B615" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C615" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="616" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B616" t="s">
-        <v>7</v>
-      </c>
-      <c r="C616" t="s">
-        <v>8</v>
+      <c r="A616" s="8"/>
+      <c r="B616" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C616" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="617" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B617" t="s">
-        <v>3</v>
-      </c>
-      <c r="C617" s="4" t="s">
-        <v>129</v>
+        <v>26</v>
+      </c>
+      <c r="C617" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="618" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B618" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C618" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="619" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B619" t="s">
-        <v>13</v>
-      </c>
-      <c r="C619" s="3">
-        <v>-1E+20</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="620" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A620" s="8"/>
-      <c r="B620" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C620" s="11" t="s">
-        <v>174</v>
+      <c r="A620" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="621" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A621" s="8"/>
-      <c r="B621" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C621" s="11" t="s">
-        <v>174</v>
+      <c r="B621" t="s">
+        <v>5</v>
+      </c>
+      <c r="C621" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="622" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B622" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C622" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
     </row>
     <row r="623" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B623" t="s">
-        <v>16</v>
-      </c>
-      <c r="C623" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="624" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>3</v>
+      </c>
+      <c r="C623" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B624" t="s">
+        <v>11</v>
+      </c>
+      <c r="C624" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="625" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A625" t="s">
-        <v>147</v>
+      <c r="B625" t="s">
+        <v>13</v>
+      </c>
+      <c r="C625" s="3">
+        <v>-1E+20</v>
       </c>
     </row>
     <row r="626" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B626" t="s">
-        <v>5</v>
-      </c>
-      <c r="C626" s="2" t="s">
-        <v>148</v>
+      <c r="A626" s="8"/>
+      <c r="B626" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C626" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="627" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B627" t="s">
-        <v>7</v>
-      </c>
-      <c r="C627" t="s">
-        <v>8</v>
+      <c r="A627" s="8"/>
+      <c r="B627" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C627" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="628" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B628" t="s">
-        <v>3</v>
-      </c>
-      <c r="C628" s="4">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C628" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="629" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B629" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C629" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="630" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B630" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C630" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="631" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A631" s="6"/>
-      <c r="B631" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C631" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="632" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="A631" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B632" t="s">
+        <v>5</v>
+      </c>
+      <c r="C632" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
     <row r="633" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A633" t="s">
-        <v>152</v>
+      <c r="B633" t="s">
+        <v>7</v>
+      </c>
+      <c r="C633" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="634" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B634" t="s">
-        <v>5</v>
-      </c>
-      <c r="C634" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C634" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="635" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B635" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C635" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B636" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C636" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A637" s="6"/>
+      <c r="B637" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C637" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A639" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B640" t="s">
+        <v>5</v>
+      </c>
+      <c r="C640" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B641" t="s">
+        <v>7</v>
+      </c>
+      <c r="C641" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="636" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B636" t="s">
-        <v>3</v>
-      </c>
-      <c r="C636" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="637" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B637" t="s">
-        <v>11</v>
-      </c>
-      <c r="C637" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="638" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B638" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C638" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="639" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B639" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C639" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="640" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A641" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="642" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B642" t="s">
-        <v>5</v>
-      </c>
-      <c r="C642" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C642" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="643" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B643" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C643" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B644" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C644" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B645" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C645" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A647" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="648" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B648" t="s">
+        <v>5</v>
+      </c>
+      <c r="C648" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B649" t="s">
+        <v>7</v>
+      </c>
+      <c r="C649" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="644" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B644" t="s">
-        <v>3</v>
-      </c>
-      <c r="C644" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="645" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B645" t="s">
-        <v>11</v>
-      </c>
-      <c r="C645" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="646" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B646" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C646" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="647" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B647" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C647" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="648" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A649" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="650" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B650" t="s">
-        <v>5</v>
-      </c>
-      <c r="C650" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C650" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="651" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B651" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C651" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B652" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C652" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="653" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B653" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C653" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="654" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A655" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="656" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B656" t="s">
+        <v>5</v>
+      </c>
+      <c r="C656" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="657" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B657" t="s">
+        <v>7</v>
+      </c>
+      <c r="C657" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="652" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B652" t="s">
-        <v>3</v>
-      </c>
-      <c r="C652" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="653" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B653" t="s">
-        <v>11</v>
-      </c>
-      <c r="C653" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="654" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B654" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C654" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="655" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B655" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C655" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="656" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A657" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="658" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B658" t="s">
-        <v>5</v>
-      </c>
-      <c r="C658" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C658" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="659" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B659" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C659" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="660" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B660" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C660" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="661" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B661" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C661" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="662" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A663" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B664" t="s">
+        <v>5</v>
+      </c>
+      <c r="C664" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B665" t="s">
+        <v>7</v>
+      </c>
+      <c r="C665" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="660" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B660" t="s">
-        <v>3</v>
-      </c>
-      <c r="C660" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="661" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B661" t="s">
-        <v>11</v>
-      </c>
-      <c r="C661" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="662" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B662" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C662" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="663" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B663" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C663" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="664" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A665" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="666" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B666" t="s">
-        <v>5</v>
-      </c>
-      <c r="C666" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C666" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="667" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B667" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C667" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B668" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C668" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B669" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C669" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A671" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B672" t="s">
+        <v>5</v>
+      </c>
+      <c r="C672" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B673" t="s">
+        <v>7</v>
+      </c>
+      <c r="C673" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="668" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B668" t="s">
-        <v>3</v>
-      </c>
-      <c r="C668" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="669" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B669" t="s">
-        <v>11</v>
-      </c>
-      <c r="C669" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="670" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B670" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C670" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="671" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B671" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C671" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="672" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A673" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="674" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B674" t="s">
-        <v>5</v>
-      </c>
-      <c r="C674" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C674" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="675" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B675" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C675" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B676" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C676" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B677" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C677" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A679" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="680" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B680" t="s">
+        <v>5</v>
+      </c>
+      <c r="C680" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="681" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B681" t="s">
+        <v>7</v>
+      </c>
+      <c r="C681" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="676" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B676" t="s">
-        <v>3</v>
-      </c>
-      <c r="C676" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="677" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B677" t="s">
-        <v>11</v>
-      </c>
-      <c r="C677" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="678" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B678" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C678" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="679" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B679" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C679" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="680" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A681" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="682" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B682" t="s">
-        <v>5</v>
-      </c>
-      <c r="C682" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C682" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="683" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B683" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C683" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B684" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C684" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B685" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C685" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="686" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A687" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B688" t="s">
+        <v>5</v>
+      </c>
+      <c r="C688" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="689" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B689" t="s">
+        <v>7</v>
+      </c>
+      <c r="C689" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="684" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B684" t="s">
-        <v>3</v>
-      </c>
-      <c r="C684" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="685" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B685" t="s">
-        <v>11</v>
-      </c>
-      <c r="C685" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="686" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B686" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C686" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="687" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B687" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C687" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="688" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A689" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="690" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B690" t="s">
-        <v>5</v>
-      </c>
-      <c r="C690" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C690" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="691" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B691" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C691" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B692" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C692" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="693" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B693" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C693" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A695" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="696" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B696" t="s">
+        <v>5</v>
+      </c>
+      <c r="C696" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="697" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B697" t="s">
+        <v>7</v>
+      </c>
+      <c r="C697" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="692" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B692" t="s">
-        <v>3</v>
-      </c>
-      <c r="C692" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="693" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B693" t="s">
-        <v>11</v>
-      </c>
-      <c r="C693" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="694" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B694" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C694" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="695" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B695" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C695" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="696" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A697" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="698" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B698" t="s">
-        <v>5</v>
-      </c>
-      <c r="C698" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C698" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="699" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B699" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C699" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="700" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B700" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C700" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="701" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B701" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C701" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="702" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A703" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B704" t="s">
+        <v>5</v>
+      </c>
+      <c r="C704" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="705" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B705" t="s">
+        <v>7</v>
+      </c>
+      <c r="C705" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="700" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B700" t="s">
-        <v>3</v>
-      </c>
-      <c r="C700" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="701" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B701" t="s">
-        <v>11</v>
-      </c>
-      <c r="C701" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="702" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B702" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C702" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="703" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B703" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C703" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="704" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A705" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="706" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B706" t="s">
-        <v>5</v>
-      </c>
-      <c r="C706" s="2" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C706" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="707" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B707" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C707" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="708" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B708" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C708" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="709" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B709" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C709" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="710" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A711" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="712" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B712" t="s">
+        <v>5</v>
+      </c>
+      <c r="C712" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B713" t="s">
+        <v>7</v>
+      </c>
+      <c r="C713" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="708" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B708" t="s">
-        <v>3</v>
-      </c>
-      <c r="C708" s="4">
+    <row r="714" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B714" t="s">
+        <v>3</v>
+      </c>
+      <c r="C714" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="709" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B709" t="s">
-        <v>11</v>
-      </c>
-      <c r="C709" t="s">
+    <row r="715" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B715" t="s">
+        <v>11</v>
+      </c>
+      <c r="C715" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="710" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B710" s="9" t="s">
+    <row r="716" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B716" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C710" s="5" t="s">
+      <c r="C716" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="711" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B711" s="14" t="s">
+    <row r="717" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B717" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C711" s="7" t="s">
+      <c r="C717" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="712" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="718" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="719" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="720" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
corrected some formatting errors in flux specific variables
</commit_message>
<xml_diff>
--- a/specific_variables/flux-components-level1.xlsx
+++ b/specific_variables/flux-components-level1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178AE73D-695E-AC47-A800-0C895C94D947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA7B7A2-A0E7-F04B-BAB5-623B2FAA2E20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="-1080" windowWidth="21480" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29100" yWindow="-1620" windowWidth="21480" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -559,10 +559,10 @@
     <t>0, 1,  2</t>
   </si>
   <si>
-    <t>0, 1,  2, 3</t>
-  </si>
-  <si>
-    <t>bad_data good_data _good_for_reasearch suspect_data_good_for_general_use suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
+    <t>bad_data good_data good_for_reasearch suspect_data_good_for_general_use suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
+  </si>
+  <si>
+    <t>0, 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
   </sheetPr>
   <dimension ref="A1:C961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A685" workbookViewId="0">
-      <selection activeCell="C692" sqref="C692:C693"/>
+    <sheetView tabSelected="1" topLeftCell="A678" workbookViewId="0">
+      <selection activeCell="C700" sqref="C700"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6054,7 +6054,7 @@
         <v>150</v>
       </c>
       <c r="C700" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="701" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6062,7 +6062,7 @@
         <v>151</v>
       </c>
       <c r="C701" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="702" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6108,7 +6108,7 @@
         <v>150</v>
       </c>
       <c r="C708" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="709" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6116,7 +6116,7 @@
         <v>151</v>
       </c>
       <c r="C709" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="710" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6162,7 +6162,7 @@
         <v>150</v>
       </c>
       <c r="C716" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="717" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6170,7 +6170,7 @@
         <v>151</v>
       </c>
       <c r="C717" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="718" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>